<commit_message>
Validated Definition class 2c and refined input space
</commit_message>
<xml_diff>
--- a/General/Def2c - variable selection.xlsx
+++ b/General/Def2c - variable selection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F5361079\GitHub\IFRS9-SICR-Definitions-Logit\General\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkLife\Analytix\Research\Dynamic-SICR\IFRS9-SICR-Definitions-Logit\General\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD342625-C8D5-4385-B5BF-1C6D340E7377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735E7B18-D665-4790-9163-3EF82B32115F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{9D6FC385-DBE1-4183-BFCB-3D03C3BB241A}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="27180" windowHeight="18885" xr2:uid="{9D6FC385-DBE1-4183-BFCB-3D03C3BB241A}"/>
   </bookViews>
   <sheets>
     <sheet name="Account-level" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>Definition</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Green-shade cells marks final inclusion as input in 'standardisation' the input space</t>
   </si>
   <si>
-    <t>slc_pmnt_method*</t>
-  </si>
-  <si>
     <t>slc_acct_pre_lim_perc_imputed</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>Real income</t>
+  </si>
+  <si>
+    <t>slc_pmnt_method</t>
   </si>
 </sst>
 </file>
@@ -235,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,16 +253,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -286,9 +280,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -326,7 +320,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -432,7 +426,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -574,7 +568,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -584,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648C4B52-8DF5-48CF-A70D-5BE671186E70}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +606,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -627,7 +621,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -648,7 +642,7 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -690,9 +684,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-      <c r="O3" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="O3" s="1"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -755,7 +747,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,14 +770,14 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -835,7 +827,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,29 +853,29 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -958,39 +950,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E828A42-20B8-48E0-BBA0-70973DBDCE8F}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11">
         <v>12</v>
       </c>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1022,81 +1014,83 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="12"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1104,14 +1098,18 @@
       <c r="E9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="F9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>